<commit_message>
check keywords function created
</commit_message>
<xml_diff>
--- a/FBOutput.xlsx
+++ b/FBOutput.xlsx
@@ -345,57 +345,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Fan Count</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Posts</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Link</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DummyBrand</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>{"data": [{"created_time": "2019-08-05T12:16:10+0000", "story": "DummyBrand updated their cover photo.", "id": "107513663924342_113193796689662"}, {"created_time": "2019-08-02T13:07:00+0000", "message": "Blogger The London Mum shares some great hamper ideas made from recycled material- we love this the idea of creating handmade crochet gifts! Very thrifty!", "id": "107513663924342_107526730589702"}, {"created_time": "2019-08-01T09:04:00+0000", "message": "Mummy Fever - we love it! Thanks for sharing the great family tree your little ones created during messy play! \nStay tuned for the new green community workshops happening soon\n\n #green #happycustomers", "id": "107513663924342_107525323923176"}, {"created_time": "2019-07-31T12:47:57+0000", "message": "We understand that things can get a little messy this summer! Extra Sensitive and environment-friendly Baby Wipes 18 Pack now available at Amazon!\n\n Shop now for the exclusive offer until 31.08.16. Subject to availability.\n\n#plasticfree #initiative", "id": "107513663924342_107517607257281"}], "paging": {"cursors": {"before": "Q2c4U1pXNTBYM0YxWlhKNVgzTjBiM0o1WDJsa0R5UXhNRGMxTVRNMk5qTTVNalF6TkRJNkxUUTNNamMyTXpRMU16RTFOak01T1RNMU1EWVBER0ZA3YVY5emRHOXllVjlwWkE4ZAk1UQTNOVEV6TmpZAek9USTBNelF5WHpFeE16RTVNemM1TmpZANE9UWTJNZAzhFZAEdsdFpRWmRTQjRLQVE9PQZDZD", "after": "Q2c4U1pXNTBYM0YxWlhKNVgzTjBiM0o1WDJsa0R5UXhNRGMxTVRNMk5qTTVNalF6TkRJNkxUY3pPRGMwTXpFM09URTFNREV6TmpFM09UUVBER0ZA3YVY5emRHOXllVjlwWkE4ZAk1UQTNOVEV6TmpZAek9USTBNelF5WHpFd056VXhOell3TnpJMU56STRNUThFZAEdsdFpRWmRRWTM5QVE9PQZDZD"}}}</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/DummyBrandKITC/</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>